<commit_message>
add streamlit ui - wip
</commit_message>
<xml_diff>
--- a/Geology Input for Petar Updated April 8th.xlsx
+++ b/Geology Input for Petar Updated April 8th.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Athos project\GeologicalCategorisation\GeoCategorisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA742D8-0074-4F8F-AE7A-C032A2F83316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94FD4C-E257-43CA-AF48-B78F8A8D7C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A66157AB-14BF-4491-9FF3-B6FED74962E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A66157AB-14BF-4491-9FF3-B6FED74962E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="101">
   <si>
     <t>Sedimentary Structures</t>
   </si>
@@ -780,7 +783,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -919,6 +922,27 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,29 +976,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1528,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F59F5A-2323-4ACD-B83A-9D2DE4AFC9F3}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,22 +1561,22 @@
       <c r="B2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="61" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1578,15 +1584,15 @@
       <c r="B3" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="55"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="62"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="69" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1610,19 +1616,19 @@
       <c r="H4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
         <v>25</v>
@@ -1640,17 +1646,17 @@
       <c r="H5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
         <v>85</v>
@@ -1666,17 +1672,17 @@
       <c r="H6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1688,17 +1694,17 @@
       <c r="H7" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="63"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1708,17 +1714,17 @@
         <v>40</v>
       </c>
       <c r="H8" s="8"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1728,17 +1734,17 @@
         <v>81</v>
       </c>
       <c r="H9" s="8"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1746,17 +1752,17 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="3"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1778,17 +1784,17 @@
       <c r="H11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9" t="s">
@@ -1806,7 +1812,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1824,7 +1830,7 @@
       <c r="O13" s="39"/>
     </row>
     <row r="14" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="63"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1844,7 +1850,7 @@
       <c r="O14" s="46"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1860,7 +1866,7 @@
       <c r="O15" s="46"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="11" t="s">
         <v>19</v>
       </c>
@@ -1882,27 +1888,27 @@
       <c r="H16" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="70" t="s">
+      <c r="J16" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="65" t="s">
+      <c r="K16" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="65" t="s">
+      <c r="L16" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="M16" s="65" t="s">
+      <c r="M16" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="N16" s="65" t="s">
+      <c r="N16" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="O16" s="54" t="s">
+      <c r="O16" s="61" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
         <v>26</v>
@@ -1922,15 +1928,15 @@
       <c r="H17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="71"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="55"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="62"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="63"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
         <v>94</v>
@@ -1966,7 +1972,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -1994,7 +2000,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="63"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2018,7 +2024,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2038,7 +2044,7 @@
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="63"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2056,7 +2062,7 @@
       <c r="O22" s="46"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63"/>
+      <c r="A23" s="70"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2072,7 +2078,7 @@
       <c r="O23" s="46"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="63"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="13" t="s">
         <v>20</v>
       </c>
@@ -2102,7 +2108,7 @@
       <c r="O24" s="46"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13" t="s">
         <v>27</v>
@@ -2126,7 +2132,7 @@
       <c r="O25" s="46"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="63"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -2144,7 +2150,7 @@
       <c r="O26" s="46"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="63"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2160,7 +2166,7 @@
       <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
+      <c r="A28" s="70"/>
       <c r="B28" s="15" t="s">
         <v>21</v>
       </c>
@@ -2190,7 +2196,7 @@
       <c r="O28" s="46"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="63"/>
+      <c r="A29" s="70"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>25</v>
@@ -2212,7 +2218,7 @@
       <c r="O29" s="46"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="64"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -2246,7 +2252,7 @@
       <c r="O31" s="46"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="66" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -2278,7 +2284,7 @@
       <c r="O32" s="46"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="60"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2304,7 +2310,7 @@
       <c r="O33" s="46"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="60"/>
+      <c r="A34" s="67"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21" t="s">
         <v>45</v>
@@ -2330,7 +2336,7 @@
       <c r="O34" s="46"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="60"/>
+      <c r="A35" s="67"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21" t="s">
         <v>46</v>
@@ -2356,7 +2362,7 @@
       <c r="O35" s="46"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="60"/>
+      <c r="A36" s="67"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
@@ -2374,7 +2380,7 @@
       <c r="O36" s="46"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="60"/>
+      <c r="A37" s="67"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2390,7 +2396,7 @@
       <c r="O37" s="46"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="60"/>
+      <c r="A38" s="67"/>
       <c r="B38" s="23" t="s">
         <v>48</v>
       </c>
@@ -2420,7 +2426,7 @@
       <c r="O38" s="46"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
+      <c r="A39" s="67"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
       <c r="D39" s="23"/>
@@ -2438,7 +2444,7 @@
       <c r="O39" s="41"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="60"/>
+      <c r="A40" s="67"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
       <c r="D40" s="23"/>
@@ -2450,7 +2456,7 @@
       <c r="H40" s="24"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="60"/>
+      <c r="A41" s="67"/>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
@@ -2466,7 +2472,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="61"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
@@ -2490,7 +2496,7 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="27" t="s">
@@ -2516,7 +2522,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29" t="s">
         <v>26</v>
@@ -2536,7 +2542,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29" t="s">
         <v>55</v>
@@ -2554,7 +2560,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29" t="s">
         <v>46</v>
@@ -2570,7 +2576,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="29"/>
       <c r="C48" s="29" t="s">
         <v>25</v>
@@ -2586,7 +2592,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29"/>
       <c r="D49" s="29"/>
@@ -2598,7 +2604,7 @@
       <c r="H49" s="28"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
+      <c r="A50" s="64"/>
       <c r="B50" s="29"/>
       <c r="C50" s="29"/>
       <c r="D50" s="29"/>
@@ -2611,7 +2617,7 @@
       <c r="K50" s="45"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2622,7 +2628,7 @@
       <c r="K51" s="45"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="30" t="s">
         <v>59</v>
       </c>
@@ -2647,7 +2653,7 @@
       <c r="K52" s="45"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30" t="s">
         <v>26</v>
@@ -2665,7 +2671,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30" t="s">
         <v>55</v>
@@ -2683,7 +2689,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="57"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30" t="s">
         <v>46</v>
@@ -2699,7 +2705,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="57"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30" t="s">
         <v>25</v>
@@ -2711,7 +2717,7 @@
       <c r="H56" s="31"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2721,7 +2727,7 @@
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="57"/>
+      <c r="A58" s="64"/>
       <c r="B58" s="32" t="s">
         <v>61</v>
       </c>
@@ -2745,7 +2751,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="57"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="32"/>
       <c r="C59" s="32" t="s">
         <v>63</v>
@@ -2767,7 +2773,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="32"/>
       <c r="C60" s="32"/>
       <c r="D60" s="32"/>
@@ -2785,7 +2791,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="57"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="32"/>
       <c r="C61" s="34"/>
       <c r="D61" s="34"/>
@@ -2799,7 +2805,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="32"/>
       <c r="C62" s="32"/>
       <c r="D62" s="32"/>
@@ -2811,7 +2817,7 @@
       <c r="H62" s="33"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="32"/>
       <c r="C63" s="32"/>
       <c r="D63" s="32"/>
@@ -2823,7 +2829,7 @@
       <c r="H63" s="33"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="32"/>
       <c r="C64" s="32"/>
       <c r="D64" s="32"/>
@@ -2835,7 +2841,7 @@
       <c r="H64" s="33"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="57"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="32"/>
       <c r="C65" s="32"/>
       <c r="D65" s="32"/>
@@ -2847,7 +2853,7 @@
       <c r="H65" s="33"/>
     </row>
     <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="58"/>
+      <c r="A66" s="65"/>
       <c r="B66" s="34"/>
       <c r="C66" s="34"/>
       <c r="D66" s="34"/>
@@ -2860,7 +2866,7 @@
     </row>
     <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="68" t="s">
+      <c r="A68" s="55" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="42" t="s">
@@ -2886,7 +2892,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="69"/>
+      <c r="A69" s="56"/>
       <c r="B69" s="42"/>
       <c r="C69" s="42"/>
       <c r="D69" s="42"/>
@@ -2897,14 +2903,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J4:Q11"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="A44:A66"/>
     <mergeCell ref="A32:A42"/>
@@ -2914,6 +2912,14 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J4:Q11"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2925,7 +2931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AED918C-4451-4981-BC80-16FB1C117AD6}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
@@ -3402,4 +3408,430 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B70DEF-5922-4A2A-9126-A879A402C3B0}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B5C6AD-CF63-42EA-A0AA-2512D5834482}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="45"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94C9F46-7880-4002-872C-B75863DCC114}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>